<commit_message>
Ajuste errores e implementacion clase locators
</commit_message>
<xml_diff>
--- a/NewExperience/bin/test/data/Data.xlsx
+++ b/NewExperience/bin/test/data/Data.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20385" windowHeight="8970" activeTab="1"/>
+    <workbookView windowWidth="18210" windowHeight="7320" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="testCases" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="contactUs" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>functionality</t>
   </si>
@@ -93,6 +94,33 @@
   </si>
   <si>
     <t>failed login</t>
+  </si>
+  <si>
+    <t>Test Description</t>
+  </si>
+  <si>
+    <t>Heading</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>filePath</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>requestSuccesful</t>
+  </si>
+  <si>
+    <t>Webmaster</t>
+  </si>
+  <si>
+    <t>/home/juan/Downloads/uu.jpg</t>
+  </si>
+  <si>
+    <t>prueba exitosa</t>
   </si>
 </sst>
 </file>
@@ -100,10 +128,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -116,12 +144,82 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,44 +235,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -183,76 +243,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,25 +307,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -309,19 +445,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -333,127 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,10 +519,75 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -514,146 +607,81 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -662,78 +690,81 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="28" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1072,90 +1103,90 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6" defaultRowHeight="12.75" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="20.6" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.8" style="2" customWidth="1"/>
-    <col min="4" max="4" width="33.4" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="20.6" style="2" customWidth="1"/>
+    <col min="1" max="2" width="20.6" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.8" style="3" customWidth="1"/>
+    <col min="4" max="4" width="33.4" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="20.6" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="25.5" spans="1:4">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="5">
         <v>1</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:4">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="22" customHeight="1" spans="1:4">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B4" s="5">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:4">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1174,8 +1205,8 @@
   <sheetPr/>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1192,7 +1223,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
@@ -1203,7 +1234,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
@@ -1221,4 +1252,64 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2">
+        <v>421806</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="juanpaosorio199@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se implementa en clase contact us steps, el consumo de datos desde un archivo excel
</commit_message>
<xml_diff>
--- a/NewExperience/bin/test/data/Data.xlsx
+++ b/NewExperience/bin/test/data/Data.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>functionality</t>
   </si>
@@ -117,10 +117,25 @@
     <t>Webmaster</t>
   </si>
   <si>
+    <t>CEOEWPQRP - 04/12/2022</t>
+  </si>
+  <si>
     <t>/home/juan/Downloads/uu.jpg</t>
   </si>
   <si>
     <t>prueba exitosa</t>
+  </si>
+  <si>
+    <t>Customer service</t>
+  </si>
+  <si>
+    <t>prueba exitosa2</t>
+  </si>
+  <si>
+    <t>prueba exitosa3</t>
+  </si>
+  <si>
+    <t>prueba exitosa4</t>
   </si>
 </sst>
 </file>
@@ -128,10 +143,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -159,6 +174,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -172,6 +194,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -182,6 +211,51 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -189,10 +263,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -204,10 +278,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -219,68 +294,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -301,19 +316,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -325,43 +448,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -373,13 +484,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -391,97 +496,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,16 +535,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -549,35 +579,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -594,16 +600,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -612,154 +627,157 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
       <alignment vertical="center"/>
@@ -1103,90 +1121,90 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6" defaultRowHeight="12.75" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="2" width="20.6" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.8" style="3" customWidth="1"/>
-    <col min="4" max="4" width="33.4" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="20.6" style="3" customWidth="1"/>
+    <col min="1" max="2" width="20.6" style="4" customWidth="1"/>
+    <col min="3" max="3" width="31.8" style="4" customWidth="1"/>
+    <col min="4" max="4" width="33.4" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="20.6" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="25.5" spans="1:4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="6">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:4">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5">
+      <c r="A3" s="6"/>
+      <c r="B3" s="6">
         <v>2</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" ht="22" customHeight="1" spans="1:4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>3</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:4">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6">
         <v>4</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1223,7 +1241,7 @@
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
@@ -1234,7 +1252,7 @@
       </c>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="B3" t="s">
@@ -1257,13 +1275,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="4" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -1286,28 +1304,88 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>421806</v>
+      <c r="D2" t="s">
+        <v>33</v>
       </c>
       <c r="E2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="1"/>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="F2" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1"/>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A5"/>
+  </mergeCells>
   <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" display="juanpaosorio199@gmail.com"/>
+    <hyperlink ref="C4" r:id="rId1" display="juanpaosorio199@gmail.com"/>
     <hyperlink ref="C2" r:id="rId1" display="juanpaosorio199@gmail.com"/>
+    <hyperlink ref="C5" r:id="rId1" display="juanpaosorio199@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Se termina de implementar toma de datos en excel para el create account page
</commit_message>
<xml_diff>
--- a/NewExperience/bin/test/data/Data.xlsx
+++ b/NewExperience/bin/test/data/Data.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18210" windowHeight="7320" activeTab="2"/>
+    <workbookView windowWidth="18210" windowHeight="7320" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="testCases" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
     <sheet name="contactUs" sheetId="3" r:id="rId3"/>
+    <sheet name="homePage" sheetId="4" r:id="rId4"/>
+    <sheet name="createAccount" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
   <si>
     <t>functionality</t>
   </si>
@@ -136,6 +138,111 @@
   </si>
   <si>
     <t>prueba exitosa4</t>
+  </si>
+  <si>
+    <t>http://automationpractice.com/index.php</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Email V</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>First Name2</t>
+  </si>
+  <si>
+    <t>Last Name2</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Address2</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>AditionalIn</t>
+  </si>
+  <si>
+    <t>HomePhone</t>
+  </si>
+  <si>
+    <t>MobilePhone</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Email caso alterno</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Osorio</t>
+  </si>
+  <si>
+    <t>juanp06@gmail.com</t>
+  </si>
+  <si>
+    <t>empresa</t>
+  </si>
+  <si>
+    <t>direccion2</t>
+  </si>
+  <si>
+    <t>Apto 508</t>
+  </si>
+  <si>
+    <t>Bogota</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Prueba1</t>
+  </si>
+  <si>
+    <t>juanpa</t>
+  </si>
+  <si>
+    <t>juanp006@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -145,8 +252,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -194,6 +301,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -226,16 +348,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -248,15 +371,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -279,14 +394,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -295,7 +402,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -316,13 +423,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -334,13 +549,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,61 +579,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,85 +591,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -525,26 +632,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -560,6 +658,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -600,16 +707,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -627,145 +734,145 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -776,11 +883,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1">
       <alignment vertical="center"/>
@@ -1224,7 +1331,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="2" outlineLevelCol="2"/>
@@ -1277,7 +1384,7 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A5"/>
     </sheetView>
   </sheetViews>
@@ -1304,13 +1411,13 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D2" t="s">
@@ -1324,11 +1431,11 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D3" t="s">
@@ -1342,11 +1449,11 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" t="s">
@@ -1360,11 +1467,11 @@
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D5" t="s">
@@ -1390,4 +1497,189 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="http://automationpractice.com/index.php"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1"/>
+  <cols>
+    <col min="20" max="20" width="11.4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>53</v>
+      </c>
+      <c r="O1" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>56</v>
+      </c>
+      <c r="R1" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2">
+        <v>31</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+      <c r="H2">
+        <v>2000</v>
+      </c>
+      <c r="I2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2">
+        <v>44444</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" t="s">
+        <v>72</v>
+      </c>
+      <c r="S2">
+        <v>7782696</v>
+      </c>
+      <c r="T2">
+        <v>3125049145</v>
+      </c>
+      <c r="U2" t="s">
+        <v>73</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="juanp06@gmail.com" tooltip="mailto:juanp06@gmail.com"/>
+    <hyperlink ref="V2" r:id="rId2" display="juanp006@gmail.com" tooltip="mailto:juanp006@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se borran comentarios en base.java y se actualiza hoja casos del archivo excel
</commit_message>
<xml_diff>
--- a/NewExperience/bin/test/data/Data.xlsx
+++ b/NewExperience/bin/test/data/Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18210" windowHeight="7320" activeTab="4"/>
+    <workbookView windowWidth="18210" windowHeight="7335"/>
   </bookViews>
   <sheets>
     <sheet name="testCases" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="85">
   <si>
     <t>functionality</t>
   </si>
@@ -62,13 +62,43 @@
     <t>The system does not allow to login successfully</t>
   </si>
   <si>
+    <t>Contact us</t>
+  </si>
+  <si>
+    <t>Make a request about a purchase, from the new experience page</t>
+  </si>
+  <si>
+    <t>The web site allows request successfully</t>
+  </si>
+  <si>
+    <t>Create failed request on the website "New Experience" in contact us module</t>
+  </si>
+  <si>
+    <t>The website displays an alert indicating that the required fields must be filled in</t>
+  </si>
+  <si>
     <t>E2E</t>
   </si>
   <si>
-    <t>Contact us</t>
+    <t>Make a complete purchase from the new experience page.</t>
+  </si>
+  <si>
+    <t>The system allows you to make the purchase successfully</t>
   </si>
   <si>
     <t>Search</t>
+  </si>
+  <si>
+    <t>Search for an existing product</t>
+  </si>
+  <si>
+    <t>The system returns articles related to the search criteria.</t>
+  </si>
+  <si>
+    <t>Perform an invalid search on the website</t>
+  </si>
+  <si>
+    <t>The system does not return results</t>
   </si>
   <si>
     <t>Email</t>
@@ -252,8 +282,8 @@
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -281,13 +311,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -310,16 +333,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -332,6 +356,21 @@
     </font>
     <font>
       <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -347,8 +386,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -362,53 +424,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,19 +453,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -447,37 +609,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,121 +657,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,6 +693,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -643,6 +718,33 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,15 +760,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -688,15 +781,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -705,105 +789,81 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -812,55 +872,55 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -869,17 +929,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -898,7 +958,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1222,8 +1297,8 @@
   <sheetPr/>
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6" defaultRowHeight="12.75" outlineLevelCol="3"/>
@@ -1275,50 +1350,103 @@
       </c>
     </row>
     <row r="4" ht="22" customHeight="1" spans="1:4">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="7">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:4">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6">
+      <c r="A5" s="7"/>
+      <c r="B5" s="7">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
-      <c r="A6" s="4" t="s">
+    <row r="6" ht="25.5" spans="1:4">
+      <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="4" t="s">
+      <c r="B6" s="8">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" s="4" t="s">
+      <c r="D6" s="8" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="7" ht="25.5" spans="1:4">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8">
+        <v>6</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" ht="25.5" hidden="1" spans="1:4">
+      <c r="A8" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="10">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" ht="25.5" hidden="1" spans="1:4">
+      <c r="A9" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="11">
+        <v>8</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" hidden="1" spans="1:4">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11">
+        <v>9</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A9:A10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1338,35 +1466,35 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1392,96 +1520,96 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
       <c r="D1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2"/>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1512,7 +1640,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -1529,7 +1657,7 @@
   <sheetPr/>
   <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -1540,87 +1668,87 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F1" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="G1" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="K1" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="M1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="N1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="O1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="P1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="Q1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="R1" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="S1" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="T1" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="U1" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="V1" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F2">
         <v>31</v>
@@ -1632,34 +1760,34 @@
         <v>2000</v>
       </c>
       <c r="I2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="K2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="L2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="M2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="N2" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="O2" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="P2">
         <v>44444</v>
       </c>
       <c r="Q2" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="R2" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="S2">
         <v>7782696</v>
@@ -1668,10 +1796,10 @@
         <v>3125049145</v>
       </c>
       <c r="U2" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>